<commit_message>
edit read file excel data
</commit_message>
<xml_diff>
--- a/pages/data_get/CLO.xlsx
+++ b/pages/data_get/CLO.xlsx
@@ -4,11 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="get_data_clo" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="get_data_course" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="get_data_clo" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,6 +433,284 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Program</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Credits</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Actions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BL2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>block1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Block chain</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Mandatory</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CLOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BLC01</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Block chain</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Block chain</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Mandatory</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CLOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BLC02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Block chain cơ bản</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Block chain</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mandatory</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Updating</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CLOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>KL01111</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Block chain</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Mandatory</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>CLOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PO001</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Khoá học CN</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Block chain</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Mandatory</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>CLOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>as1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Block chain</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Mandatory</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>CLOs</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>